<commit_message>
Crude graft of power2 task into new excel lab
</commit_message>
<xml_diff>
--- a/lab/spreadsheets/1 - 152/tankvolume.xlsx
+++ b/lab/spreadsheets/1 - 152/tankvolume.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Local\comp152\lab\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Local\comp152\lab\spreadsheets\1 - 152\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,13 +50,7 @@
     <t>(sec)</t>
   </si>
   <si>
-    <t>(m3)</t>
-  </si>
-  <si>
     <t>(m)</t>
-  </si>
-  <si>
-    <t>m2</t>
   </si>
   <si>
     <r>
@@ -100,12 +94,54 @@
       <t>/sec</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>(m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +152,14 @@
     <font>
       <vertAlign val="superscript"/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -142,8 +186,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,13 +506,16 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -479,7 +527,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
@@ -490,10 +538,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -501,7 +549,7 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -515,15 +563,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>